<commit_message>
Run Tests With Cucumber
</commit_message>
<xml_diff>
--- a/src/test/java/data/SubscriptionData.xlsx
+++ b/src/test/java/data/SubscriptionData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Self Development\tasks\testCrewTask\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23113F88-3BC5-4CD2-B48F-6F9D7918C42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3AA71E-18F6-4837-B846-8E2753E79C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KSA" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +399,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -429,6 +429,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -437,7 +438,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,6 +493,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -500,7 +502,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>